<commit_message>
Update ICAREdata DSTU2 IG to v0.1.2
</commit_message>
<xml_diff>
--- a/docs/icare/icare-CarePlanWithReview.xlsx
+++ b/docs/icare/icare-CarePlanWithReview.xlsx
@@ -239,7 +239,7 @@
     <t>sourcesystem</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-SourceSystem-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-SourceSystem-extension}
 </t>
   </si>
   <si>
@@ -430,7 +430,7 @@
     <t>basedon</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-BasedOn-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-BasedOn-extension}
 </t>
   </si>
   <si>
@@ -461,7 +461,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition should be version specific.  This will ideally be the URI for the Resource Profile defining the extension, with the code for the extension after a #.</t>
   </si>
   <si>
-    <t>http://icaredata.org/icare/StructureDefinition/obf-BasedOn-extension</t>
+    <t>http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-BasedOn-extension</t>
   </si>
   <si>
     <t>Extension.url</t>
@@ -470,7 +470,7 @@
     <t>CarePlan.extension.valueReference</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://icaredata.org/icare/StructureDefinition/obf-CarePlan)
+    <t xml:space="preserve">Reference(http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-CarePlan)
 </t>
   </si>
   <si>
@@ -486,7 +486,7 @@
     <t>statementdatetime</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-StatementDateTime-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-StatementDateTime-extension}
 </t>
   </si>
   <si>
@@ -496,7 +496,7 @@
     <t>reasoncode</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-ReasonCode-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-ReasonCode-extension}
 </t>
   </si>
   <si>
@@ -507,7 +507,7 @@
     <t>careplanreplaces</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-CarePlanReplaces-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-CarePlanReplaces-extension}
 </t>
   </si>
   <si>
@@ -517,7 +517,7 @@
     <t>careplanpartof</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-CarePlanPartOf-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-CarePlanPartOf-extension}
 </t>
   </si>
   <si>
@@ -527,7 +527,7 @@
     <t>requestintent</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-RequestIntent-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-RequestIntent-extension}
 </t>
   </si>
   <si>
@@ -537,7 +537,7 @@
     <t>title</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/obf-datatype-Title-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/obf-datatype-Title-extension}
 </t>
   </si>
   <si>
@@ -547,7 +547,7 @@
     <t>review</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://icaredata.org/icare/StructureDefinition/icare-Review-extension}
+    <t xml:space="preserve">Extension {http://mcodeinitiative.org/codex/us/icare/StructureDefinition/icare-Review-extension}
 </t>
   </si>
   <si>

</xml_diff>